<commit_message>
Added logging frequencies through GTK-NET, added matlab script for logged frequencies, added two bus test system for finding otpimal DLAA attack vector
</commit_message>
<xml_diff>
--- a/LFC with network/Loads Description.xlsx
+++ b/LFC with network/Loads Description.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kaust-my.sharepoint.com/personal/forystmj_kaust_edu_sa/Documents/Documents/RSCAD/RTDS_USER_FX/fileman/IEEE 39 Bus Power System_Michal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forystmj\Documents\RSCAD\RTDS_USER_FX\fileman\LFC with network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{948712B4-9F1A-47A9-91A5-2D0C1E39BBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{034F2106-9CDD-4746-8D97-88B70850EAF2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{25F43F66-12A4-441C-BEEC-B33793F70A62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="120">
   <si>
     <t>Bus</t>
   </si>
@@ -229,13 +229,181 @@
   </si>
   <si>
     <t>9-29</t>
+  </si>
+  <si>
+    <t>Len (km)</t>
+  </si>
+  <si>
+    <t>X (Ohm/km)</t>
+  </si>
+  <si>
+    <t>R (Ohm/km)</t>
+  </si>
+  <si>
+    <t>Bus 2</t>
+  </si>
+  <si>
+    <t>Bus 1</t>
+  </si>
+  <si>
+    <t>Line num</t>
+  </si>
+  <si>
+    <t>R (Ohm)</t>
+  </si>
+  <si>
+    <t>X(Ohm)</t>
+  </si>
+  <si>
+    <t>Impedance</t>
+  </si>
+  <si>
+    <t>Admittance (imag)</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>T11</t>
+  </si>
+  <si>
+    <t>T12</t>
+  </si>
+  <si>
+    <t>T13</t>
+  </si>
+  <si>
+    <t>T14</t>
+  </si>
+  <si>
+    <t>T15</t>
+  </si>
+  <si>
+    <t>T16</t>
+  </si>
+  <si>
+    <t>T17</t>
+  </si>
+  <si>
+    <t>T18</t>
+  </si>
+  <si>
+    <t>T19</t>
+  </si>
+  <si>
+    <t>T20</t>
+  </si>
+  <si>
+    <t>T21</t>
+  </si>
+  <si>
+    <t>T22</t>
+  </si>
+  <si>
+    <t>T23</t>
+  </si>
+  <si>
+    <t>T24</t>
+  </si>
+  <si>
+    <t>T25</t>
+  </si>
+  <si>
+    <t>T26</t>
+  </si>
+  <si>
+    <t>T27</t>
+  </si>
+  <si>
+    <t>T28</t>
+  </si>
+  <si>
+    <t>T29</t>
+  </si>
+  <si>
+    <t>T30</t>
+  </si>
+  <si>
+    <t>T31</t>
+  </si>
+  <si>
+    <t>T32</t>
+  </si>
+  <si>
+    <t>T33</t>
+  </si>
+  <si>
+    <t>T37</t>
+  </si>
+  <si>
+    <t>T38</t>
+  </si>
+  <si>
+    <t>T39</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>G8</t>
+  </si>
+  <si>
+    <t>G9</t>
+  </si>
+  <si>
+    <t>G10</t>
+  </si>
+  <si>
+    <t>Tap change</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -610,7 +778,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -703,6 +871,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -748,8 +919,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1088,41 +1257,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B6E1A9F-C9C1-466A-B246-0C3C0DC4529A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE59"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="8.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.75" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.4140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.75" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:31" ht="14.5" thickBot="1">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -1148,31 +1317,31 @@
       <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="46" t="s">
+      <c r="K1" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="48"/>
-      <c r="V1" s="46" t="s">
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="51"/>
+      <c r="V1" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="48"/>
-    </row>
-    <row r="2" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="59" t="s">
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="51"/>
+    </row>
+    <row r="2" spans="1:31" ht="14.5" thickBot="1">
+      <c r="A2" s="62" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="15">
@@ -1258,8 +1427,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A3" s="57"/>
+    <row r="3" spans="1:31">
+      <c r="A3" s="60"/>
       <c r="B3" s="15">
         <v>16</v>
       </c>
@@ -1357,8 +1526,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A4" s="57"/>
+    <row r="4" spans="1:31">
+      <c r="A4" s="60"/>
       <c r="B4" s="15">
         <v>20</v>
       </c>
@@ -1406,17 +1575,17 @@
         <f>IF(EXACT(N4,_xlfn.XLOOKUP(K4,$B$2:$B$21,$E$2:$E$21)), TRUE, FALSE)</f>
         <v>1</v>
       </c>
-      <c r="P4" s="49">
+      <c r="P4" s="52">
         <v>30</v>
       </c>
-      <c r="Q4" s="53">
+      <c r="Q4" s="56">
         <v>0.1</v>
       </c>
-      <c r="R4" s="49">
+      <c r="R4" s="52">
         <f>Q4*$C$23</f>
         <v>608.79</v>
       </c>
-      <c r="S4" s="51">
+      <c r="S4" s="54">
         <v>1</v>
       </c>
       <c r="V4" s="13">
@@ -1443,8 +1612,8 @@
       <c r="AC4" s="11"/>
       <c r="AD4" s="19"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A5" s="57"/>
+    <row r="5" spans="1:31">
+      <c r="A5" s="60"/>
       <c r="B5" s="15">
         <v>21</v>
       </c>
@@ -1492,10 +1661,10 @@
         <f>IF(EXACT(N5,_xlfn.XLOOKUP(K5,$B$2:$B$21,$E$2:$E$21)), TRUE, FALSE)</f>
         <v>0</v>
       </c>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="54"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="52"/>
+      <c r="P5" s="53"/>
+      <c r="Q5" s="57"/>
+      <c r="R5" s="53"/>
+      <c r="S5" s="55"/>
       <c r="T5" s="20"/>
       <c r="V5" s="30">
         <v>3</v>
@@ -1533,8 +1702,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A6" s="57"/>
+    <row r="6" spans="1:31">
+      <c r="A6" s="60"/>
       <c r="B6" s="15">
         <v>23</v>
       </c>
@@ -1582,17 +1751,17 @@
         <f t="shared" ref="O6:O18" si="10">IF(EXACT(N6,_xlfn.XLOOKUP(K6,$B$2:$B$21,$E$2:$E$21)), TRUE, FALSE)</f>
         <v>1</v>
       </c>
-      <c r="P6" s="49">
+      <c r="P6" s="52">
         <v>30</v>
       </c>
-      <c r="Q6" s="53">
+      <c r="Q6" s="56">
         <v>0.1</v>
       </c>
-      <c r="R6" s="49">
+      <c r="R6" s="52">
         <f>Q6*$C$23</f>
         <v>608.79</v>
       </c>
-      <c r="S6" s="51" t="s">
+      <c r="S6" s="54" t="s">
         <v>20</v>
       </c>
       <c r="V6" s="24">
@@ -1620,8 +1789,8 @@
       <c r="AD6" s="11"/>
       <c r="AE6" s="20"/>
     </row>
-    <row r="7" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="57"/>
+    <row r="7" spans="1:31" ht="14.5" thickBot="1">
+      <c r="A7" s="60"/>
       <c r="B7" s="15">
         <v>24</v>
       </c>
@@ -1669,10 +1838,10 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="54"/>
-      <c r="R7" s="50"/>
-      <c r="S7" s="52"/>
+      <c r="P7" s="53"/>
+      <c r="Q7" s="57"/>
+      <c r="R7" s="53"/>
+      <c r="S7" s="55"/>
       <c r="V7" s="39">
         <v>4</v>
       </c>
@@ -1709,8 +1878,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="58"/>
+    <row r="8" spans="1:31" ht="14.5" thickBot="1">
+      <c r="A8" s="61"/>
       <c r="B8" s="5" t="s">
         <v>4</v>
       </c>
@@ -1761,17 +1930,17 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P8" s="49">
+      <c r="P8" s="52">
         <v>30</v>
       </c>
-      <c r="Q8" s="53">
+      <c r="Q8" s="56">
         <v>0.2</v>
       </c>
-      <c r="R8" s="49">
+      <c r="R8" s="52">
         <f>Q8*$C$23</f>
         <v>1217.58</v>
       </c>
-      <c r="S8" s="51" t="s">
+      <c r="S8" s="54" t="s">
         <v>20</v>
       </c>
       <c r="T8" s="9"/>
@@ -1811,8 +1980,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A9" s="57" t="s">
+    <row r="9" spans="1:31">
+      <c r="A9" s="60" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="15">
@@ -1863,10 +2032,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="60"/>
-      <c r="R9" s="55"/>
-      <c r="S9" s="56"/>
+      <c r="P9" s="58"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="58"/>
+      <c r="S9" s="59"/>
       <c r="T9" s="9"/>
       <c r="V9" s="20">
         <v>27</v>
@@ -1889,8 +2058,8 @@
       </c>
       <c r="AD9" s="34"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A10" s="57"/>
+    <row r="10" spans="1:31">
+      <c r="A10" s="60"/>
       <c r="B10" s="15">
         <v>18</v>
       </c>
@@ -1938,10 +2107,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P10" s="55"/>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="55"/>
-      <c r="S10" s="56"/>
+      <c r="P10" s="58"/>
+      <c r="Q10" s="63"/>
+      <c r="R10" s="58"/>
+      <c r="S10" s="59"/>
       <c r="T10" s="9"/>
       <c r="V10" s="24">
         <v>29</v>
@@ -1967,8 +2136,8 @@
       <c r="AC10" s="22"/>
       <c r="AD10" s="42"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A11" s="57"/>
+    <row r="11" spans="1:31">
+      <c r="A11" s="60"/>
       <c r="B11" s="15">
         <v>25</v>
       </c>
@@ -2016,10 +2185,10 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P11" s="55"/>
-      <c r="Q11" s="60"/>
-      <c r="R11" s="50"/>
-      <c r="S11" s="56"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="63"/>
+      <c r="R11" s="53"/>
+      <c r="S11" s="59"/>
       <c r="T11" s="9"/>
       <c r="V11" s="30">
         <v>16</v>
@@ -2057,8 +2226,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A12" s="57"/>
+    <row r="12" spans="1:31">
+      <c r="A12" s="60"/>
       <c r="B12" s="15">
         <v>26</v>
       </c>
@@ -2106,17 +2275,17 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P12" s="49">
+      <c r="P12" s="52">
         <v>30</v>
       </c>
-      <c r="Q12" s="53">
+      <c r="Q12" s="56">
         <v>0.5</v>
       </c>
-      <c r="R12" s="49">
+      <c r="R12" s="52">
         <f t="shared" ref="R12" si="15">Q12*$C$23</f>
         <v>3043.95</v>
       </c>
-      <c r="S12" s="51" t="s">
+      <c r="S12" s="54" t="s">
         <v>21</v>
       </c>
       <c r="V12" s="20">
@@ -2140,8 +2309,8 @@
       </c>
       <c r="AE12" s="20"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A13" s="57"/>
+    <row r="13" spans="1:31">
+      <c r="A13" s="60"/>
       <c r="B13" s="15">
         <v>27</v>
       </c>
@@ -2189,10 +2358,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="60"/>
-      <c r="R13" s="55"/>
-      <c r="S13" s="56"/>
+      <c r="P13" s="58"/>
+      <c r="Q13" s="63"/>
+      <c r="R13" s="58"/>
+      <c r="S13" s="59"/>
       <c r="V13" s="24">
         <v>24</v>
       </c>
@@ -2217,8 +2386,8 @@
       <c r="AC13" s="22"/>
       <c r="AD13" s="42"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A14" s="57"/>
+    <row r="14" spans="1:31">
+      <c r="A14" s="60"/>
       <c r="B14" s="15">
         <v>28</v>
       </c>
@@ -2266,10 +2435,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P14" s="55"/>
-      <c r="Q14" s="60"/>
-      <c r="R14" s="55"/>
-      <c r="S14" s="56"/>
+      <c r="P14" s="58"/>
+      <c r="Q14" s="63"/>
+      <c r="R14" s="58"/>
+      <c r="S14" s="59"/>
       <c r="V14" s="30">
         <v>27</v>
       </c>
@@ -2306,8 +2475,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="57"/>
+    <row r="15" spans="1:31" ht="14.5" thickBot="1">
+      <c r="A15" s="60"/>
       <c r="B15" s="15">
         <v>29</v>
       </c>
@@ -2355,10 +2524,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P15" s="55"/>
-      <c r="Q15" s="60"/>
-      <c r="R15" s="55"/>
-      <c r="S15" s="56"/>
+      <c r="P15" s="58"/>
+      <c r="Q15" s="63"/>
+      <c r="R15" s="58"/>
+      <c r="S15" s="59"/>
       <c r="V15" s="24">
         <v>4</v>
       </c>
@@ -2383,8 +2552,8 @@
       <c r="AC15" s="22"/>
       <c r="AD15" s="42"/>
     </row>
-    <row r="16" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="58"/>
+    <row r="16" spans="1:31" ht="14.5" thickBot="1">
+      <c r="A16" s="61"/>
       <c r="B16" s="5" t="s">
         <v>4</v>
       </c>
@@ -2435,10 +2604,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P16" s="55"/>
-      <c r="Q16" s="60"/>
-      <c r="R16" s="55"/>
-      <c r="S16" s="56"/>
+      <c r="P16" s="58"/>
+      <c r="Q16" s="63"/>
+      <c r="R16" s="58"/>
+      <c r="S16" s="59"/>
       <c r="V16" s="30">
         <v>16</v>
       </c>
@@ -2475,8 +2644,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A17" s="59" t="s">
+    <row r="17" spans="1:31">
+      <c r="A17" s="62" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="15">
@@ -2526,10 +2695,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P17" s="55"/>
-      <c r="Q17" s="60"/>
-      <c r="R17" s="55"/>
-      <c r="S17" s="56"/>
+      <c r="P17" s="58"/>
+      <c r="Q17" s="63"/>
+      <c r="R17" s="58"/>
+      <c r="S17" s="59"/>
       <c r="V17" s="20">
         <v>27</v>
       </c>
@@ -2554,8 +2723,8 @@
       <c r="AC17" s="21"/>
       <c r="AD17" s="33"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A18" s="57"/>
+    <row r="18" spans="1:31">
+      <c r="A18" s="60"/>
       <c r="B18" s="15">
         <v>7</v>
       </c>
@@ -2603,10 +2772,10 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P18" s="50"/>
-      <c r="Q18" s="54"/>
-      <c r="R18" s="50"/>
-      <c r="S18" s="52"/>
+      <c r="P18" s="53"/>
+      <c r="Q18" s="57"/>
+      <c r="R18" s="53"/>
+      <c r="S18" s="55"/>
       <c r="V18" s="24">
         <v>39</v>
       </c>
@@ -2631,8 +2800,8 @@
       <c r="AC18" s="11"/>
       <c r="AD18" s="19"/>
     </row>
-    <row r="19" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="57"/>
+    <row r="19" spans="1:31" ht="14.5" thickBot="1">
+      <c r="A19" s="60"/>
       <c r="B19" s="15">
         <v>8</v>
       </c>
@@ -2663,8 +2832,8 @@
       </c>
       <c r="N19" s="29"/>
     </row>
-    <row r="20" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="57"/>
+    <row r="20" spans="1:31" ht="14.5" thickBot="1">
+      <c r="A20" s="60"/>
       <c r="B20" s="15">
         <v>12</v>
       </c>
@@ -2712,33 +2881,33 @@
         <f>IF(EXACT(N20,_xlfn.XLOOKUP(K20,$B$2:$B$21,$D$2:$D$21)), TRUE, FALSE)</f>
         <v>1</v>
       </c>
-      <c r="P20" s="49">
+      <c r="P20" s="52">
         <v>30</v>
       </c>
-      <c r="Q20" s="53">
+      <c r="Q20" s="56">
         <v>-0.05</v>
       </c>
-      <c r="R20" s="49">
+      <c r="R20" s="52">
         <f>Q20*$C$23</f>
         <v>-304.39499999999998</v>
       </c>
-      <c r="S20" s="51">
-        <v>1</v>
-      </c>
-      <c r="V20" s="46" t="s">
+      <c r="S20" s="54">
+        <v>1</v>
+      </c>
+      <c r="V20" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="W20" s="47"/>
-      <c r="X20" s="47"/>
-      <c r="Y20" s="47"/>
-      <c r="Z20" s="47"/>
-      <c r="AA20" s="47"/>
-      <c r="AB20" s="47"/>
-      <c r="AC20" s="47"/>
-      <c r="AD20" s="48"/>
-    </row>
-    <row r="21" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="57"/>
+      <c r="W20" s="50"/>
+      <c r="X20" s="50"/>
+      <c r="Y20" s="50"/>
+      <c r="Z20" s="50"/>
+      <c r="AA20" s="50"/>
+      <c r="AB20" s="50"/>
+      <c r="AC20" s="50"/>
+      <c r="AD20" s="51"/>
+    </row>
+    <row r="21" spans="1:31" ht="14.5" thickBot="1">
+      <c r="A21" s="60"/>
       <c r="B21" s="15">
         <v>39</v>
       </c>
@@ -2786,10 +2955,10 @@
         <f t="shared" ref="O21:O55" si="25">IF(EXACT(N21,_xlfn.XLOOKUP(K21,$B$2:$B$21,$D$2:$D$21)), TRUE, FALSE)</f>
         <v>0</v>
       </c>
-      <c r="P21" s="50"/>
-      <c r="Q21" s="54"/>
-      <c r="R21" s="50"/>
-      <c r="S21" s="52"/>
+      <c r="P21" s="53"/>
+      <c r="Q21" s="57"/>
+      <c r="R21" s="53"/>
+      <c r="S21" s="55"/>
       <c r="U21" s="21" t="s">
         <v>26</v>
       </c>
@@ -2821,8 +2990,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="58"/>
+    <row r="22" spans="1:31" ht="14.5" thickBot="1">
+      <c r="A22" s="61"/>
       <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
@@ -2873,17 +3042,17 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P22" s="49">
+      <c r="P22" s="52">
         <v>30</v>
       </c>
-      <c r="Q22" s="53">
+      <c r="Q22" s="56">
         <v>-0.1</v>
       </c>
-      <c r="R22" s="49">
+      <c r="R22" s="52">
         <f>Q22*$C$23</f>
         <v>-608.79</v>
       </c>
-      <c r="S22" s="51">
+      <c r="S22" s="54">
         <v>1</v>
       </c>
       <c r="U22" t="s">
@@ -2925,7 +3094,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:31" ht="14.5" thickBot="1">
       <c r="A23" s="6"/>
       <c r="B23" s="10" t="s">
         <v>8</v>
@@ -2977,10 +3146,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P23" s="55"/>
-      <c r="Q23" s="60"/>
-      <c r="R23" s="55"/>
-      <c r="S23" s="56"/>
+      <c r="P23" s="58"/>
+      <c r="Q23" s="63"/>
+      <c r="R23" s="58"/>
+      <c r="S23" s="59"/>
       <c r="U23" t="s">
         <v>24</v>
       </c>
@@ -3015,7 +3184,7 @@
       </c>
       <c r="AD23" s="33"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:31">
       <c r="K24" s="24">
         <v>20</v>
       </c>
@@ -3035,10 +3204,10 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="P24" s="50"/>
-      <c r="Q24" s="54"/>
-      <c r="R24" s="50"/>
-      <c r="S24" s="52"/>
+      <c r="P24" s="53"/>
+      <c r="Q24" s="57"/>
+      <c r="R24" s="53"/>
+      <c r="S24" s="55"/>
       <c r="U24" t="s">
         <v>25</v>
       </c>
@@ -3066,7 +3235,7 @@
       <c r="AC24" s="11"/>
       <c r="AD24" s="19"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:31">
       <c r="K25" s="30">
         <v>16</v>
       </c>
@@ -3086,17 +3255,17 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P25" s="49">
+      <c r="P25" s="52">
         <v>30</v>
       </c>
-      <c r="Q25" s="53">
+      <c r="Q25" s="56">
         <v>-0.1</v>
       </c>
-      <c r="R25" s="49">
+      <c r="R25" s="52">
         <f>Q25*$C$23</f>
         <v>-608.79</v>
       </c>
-      <c r="S25" s="51" t="s">
+      <c r="S25" s="54" t="s">
         <v>20</v>
       </c>
       <c r="U25" t="s">
@@ -3138,7 +3307,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:31">
       <c r="K26" s="20">
         <v>24</v>
       </c>
@@ -3158,10 +3327,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P26" s="55"/>
-      <c r="Q26" s="60"/>
-      <c r="R26" s="55"/>
-      <c r="S26" s="56"/>
+      <c r="P26" s="58"/>
+      <c r="Q26" s="63"/>
+      <c r="R26" s="58"/>
+      <c r="S26" s="59"/>
       <c r="U26" t="s">
         <v>24</v>
       </c>
@@ -3196,7 +3365,7 @@
       </c>
       <c r="AD26" s="33"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:31">
       <c r="K27" s="20">
         <v>3</v>
       </c>
@@ -3216,10 +3385,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P27" s="55"/>
-      <c r="Q27" s="60"/>
-      <c r="R27" s="55"/>
-      <c r="S27" s="56"/>
+      <c r="P27" s="58"/>
+      <c r="Q27" s="63"/>
+      <c r="R27" s="58"/>
+      <c r="S27" s="59"/>
       <c r="U27" t="s">
         <v>25</v>
       </c>
@@ -3247,7 +3416,7 @@
       <c r="AC27" s="11"/>
       <c r="AD27" s="19"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:31">
       <c r="K28" s="24">
         <v>27</v>
       </c>
@@ -3267,10 +3436,10 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="P28" s="50"/>
-      <c r="Q28" s="54"/>
-      <c r="R28" s="50"/>
-      <c r="S28" s="52"/>
+      <c r="P28" s="53"/>
+      <c r="Q28" s="57"/>
+      <c r="R28" s="53"/>
+      <c r="S28" s="55"/>
       <c r="U28" t="s">
         <v>27</v>
       </c>
@@ -3310,7 +3479,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:31">
       <c r="K29" s="30">
         <v>15</v>
       </c>
@@ -3330,17 +3499,17 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P29" s="49">
+      <c r="P29" s="52">
         <v>30</v>
       </c>
-      <c r="Q29" s="53">
+      <c r="Q29" s="56">
         <v>-0.2</v>
       </c>
-      <c r="R29" s="49">
+      <c r="R29" s="52">
         <f>Q29*$C$23</f>
         <v>-1217.58</v>
       </c>
-      <c r="S29" s="51" t="s">
+      <c r="S29" s="54" t="s">
         <v>20</v>
       </c>
       <c r="U29" t="s">
@@ -3377,7 +3546,7 @@
       </c>
       <c r="AD29" s="19"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:31">
       <c r="K30" s="20">
         <v>16</v>
       </c>
@@ -3397,10 +3566,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P30" s="55"/>
-      <c r="Q30" s="60"/>
-      <c r="R30" s="55"/>
-      <c r="S30" s="56"/>
+      <c r="P30" s="58"/>
+      <c r="Q30" s="63"/>
+      <c r="R30" s="58"/>
+      <c r="S30" s="59"/>
       <c r="U30" t="s">
         <v>27</v>
       </c>
@@ -3440,7 +3609,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:31">
       <c r="K31" s="20">
         <v>20</v>
       </c>
@@ -3460,10 +3629,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P31" s="55"/>
-      <c r="Q31" s="60"/>
-      <c r="R31" s="55"/>
-      <c r="S31" s="56"/>
+      <c r="P31" s="58"/>
+      <c r="Q31" s="63"/>
+      <c r="R31" s="58"/>
+      <c r="S31" s="59"/>
       <c r="U31" t="s">
         <v>25</v>
       </c>
@@ -3491,7 +3660,7 @@
       <c r="AC31" s="21"/>
       <c r="AD31" s="33"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:31">
       <c r="K32" s="20">
         <v>21</v>
       </c>
@@ -3511,10 +3680,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P32" s="55"/>
-      <c r="Q32" s="60"/>
-      <c r="R32" s="55"/>
-      <c r="S32" s="56"/>
+      <c r="P32" s="58"/>
+      <c r="Q32" s="63"/>
+      <c r="R32" s="58"/>
+      <c r="S32" s="59"/>
       <c r="U32" t="s">
         <v>24</v>
       </c>
@@ -3549,7 +3718,7 @@
       </c>
       <c r="AD32" s="33"/>
     </row>
-    <row r="33" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="33" spans="11:31">
       <c r="K33" s="20">
         <v>3</v>
       </c>
@@ -3569,10 +3738,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P33" s="55"/>
-      <c r="Q33" s="60"/>
-      <c r="R33" s="55"/>
-      <c r="S33" s="56"/>
+      <c r="P33" s="58"/>
+      <c r="Q33" s="63"/>
+      <c r="R33" s="58"/>
+      <c r="S33" s="59"/>
       <c r="U33" t="s">
         <v>25</v>
       </c>
@@ -3600,7 +3769,7 @@
       <c r="AC33" s="21"/>
       <c r="AD33" s="33"/>
     </row>
-    <row r="34" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="34" spans="11:31">
       <c r="K34" s="20">
         <v>18</v>
       </c>
@@ -3620,10 +3789,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P34" s="55"/>
-      <c r="Q34" s="60"/>
-      <c r="R34" s="55"/>
-      <c r="S34" s="56"/>
+      <c r="P34" s="58"/>
+      <c r="Q34" s="63"/>
+      <c r="R34" s="58"/>
+      <c r="S34" s="59"/>
       <c r="U34" t="s">
         <v>25</v>
       </c>
@@ -3651,7 +3820,7 @@
       <c r="AC34" s="21"/>
       <c r="AD34" s="33"/>
     </row>
-    <row r="35" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="35" spans="11:31">
       <c r="K35" s="20">
         <v>25</v>
       </c>
@@ -3671,10 +3840,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P35" s="55"/>
-      <c r="Q35" s="60"/>
-      <c r="R35" s="55"/>
-      <c r="S35" s="56"/>
+      <c r="P35" s="58"/>
+      <c r="Q35" s="63"/>
+      <c r="R35" s="58"/>
+      <c r="S35" s="59"/>
       <c r="U35" t="s">
         <v>24</v>
       </c>
@@ -3709,7 +3878,7 @@
       </c>
       <c r="AD35" s="33"/>
     </row>
-    <row r="36" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="36" spans="11:31">
       <c r="K36" s="20">
         <v>26</v>
       </c>
@@ -3729,10 +3898,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P36" s="55"/>
-      <c r="Q36" s="60"/>
-      <c r="R36" s="55"/>
-      <c r="S36" s="56"/>
+      <c r="P36" s="58"/>
+      <c r="Q36" s="63"/>
+      <c r="R36" s="58"/>
+      <c r="S36" s="59"/>
       <c r="U36" t="s">
         <v>25</v>
       </c>
@@ -3760,7 +3929,7 @@
       <c r="AC36" s="21"/>
       <c r="AD36" s="33"/>
     </row>
-    <row r="37" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="37" spans="11:31">
       <c r="K37" s="24">
         <v>27</v>
       </c>
@@ -3780,10 +3949,10 @@
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="P37" s="50"/>
-      <c r="Q37" s="54"/>
-      <c r="R37" s="50"/>
-      <c r="S37" s="52"/>
+      <c r="P37" s="53"/>
+      <c r="Q37" s="57"/>
+      <c r="R37" s="53"/>
+      <c r="S37" s="55"/>
       <c r="U37" t="s">
         <v>25</v>
       </c>
@@ -3811,7 +3980,7 @@
       <c r="AC37" s="11"/>
       <c r="AD37" s="19"/>
     </row>
-    <row r="38" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="38" spans="11:31">
       <c r="K38" s="30">
         <v>15</v>
       </c>
@@ -3831,17 +4000,17 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P38" s="49">
+      <c r="P38" s="52">
         <v>30</v>
       </c>
-      <c r="Q38" s="53">
+      <c r="Q38" s="56">
         <v>-0.5</v>
       </c>
-      <c r="R38" s="49">
+      <c r="R38" s="52">
         <f>Q38*$C$23</f>
         <v>-3043.95</v>
       </c>
-      <c r="S38" s="51" t="s">
+      <c r="S38" s="54" t="s">
         <v>21</v>
       </c>
       <c r="U38" t="s">
@@ -3883,7 +4052,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="39" spans="11:31">
       <c r="K39" s="20">
         <v>16</v>
       </c>
@@ -3903,10 +4072,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P39" s="55"/>
-      <c r="Q39" s="60"/>
-      <c r="R39" s="55"/>
-      <c r="S39" s="56"/>
+      <c r="P39" s="58"/>
+      <c r="Q39" s="63"/>
+      <c r="R39" s="58"/>
+      <c r="S39" s="59"/>
       <c r="U39" t="s">
         <v>25</v>
       </c>
@@ -3934,7 +4103,7 @@
       <c r="AC39" s="21"/>
       <c r="AD39" s="33"/>
     </row>
-    <row r="40" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="40" spans="11:31">
       <c r="K40" s="20">
         <v>20</v>
       </c>
@@ -3954,10 +4123,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P40" s="55"/>
-      <c r="Q40" s="60"/>
-      <c r="R40" s="55"/>
-      <c r="S40" s="56"/>
+      <c r="P40" s="58"/>
+      <c r="Q40" s="63"/>
+      <c r="R40" s="58"/>
+      <c r="S40" s="59"/>
       <c r="U40" t="s">
         <v>24</v>
       </c>
@@ -3992,7 +4161,7 @@
       </c>
       <c r="AD40" s="33"/>
     </row>
-    <row r="41" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="41" spans="11:31">
       <c r="K41" s="20">
         <v>21</v>
       </c>
@@ -4012,10 +4181,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P41" s="55"/>
-      <c r="Q41" s="60"/>
-      <c r="R41" s="55"/>
-      <c r="S41" s="56"/>
+      <c r="P41" s="58"/>
+      <c r="Q41" s="63"/>
+      <c r="R41" s="58"/>
+      <c r="S41" s="59"/>
       <c r="U41" t="s">
         <v>25</v>
       </c>
@@ -4043,7 +4212,7 @@
       <c r="AC41" s="21"/>
       <c r="AD41" s="33"/>
     </row>
-    <row r="42" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="42" spans="11:31">
       <c r="K42" s="20">
         <v>23</v>
       </c>
@@ -4063,10 +4232,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P42" s="55"/>
-      <c r="Q42" s="60"/>
-      <c r="R42" s="55"/>
-      <c r="S42" s="56"/>
+      <c r="P42" s="58"/>
+      <c r="Q42" s="63"/>
+      <c r="R42" s="58"/>
+      <c r="S42" s="59"/>
       <c r="U42" t="s">
         <v>24</v>
       </c>
@@ -4101,7 +4270,7 @@
       </c>
       <c r="AD42" s="33"/>
     </row>
-    <row r="43" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="43" spans="11:31">
       <c r="K43" s="20">
         <v>24</v>
       </c>
@@ -4121,10 +4290,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P43" s="55"/>
-      <c r="Q43" s="60"/>
-      <c r="R43" s="55"/>
-      <c r="S43" s="56"/>
+      <c r="P43" s="58"/>
+      <c r="Q43" s="63"/>
+      <c r="R43" s="58"/>
+      <c r="S43" s="59"/>
       <c r="U43" t="s">
         <v>25</v>
       </c>
@@ -4152,7 +4321,7 @@
       <c r="AC43" s="21"/>
       <c r="AD43" s="33"/>
     </row>
-    <row r="44" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="44" spans="11:31">
       <c r="K44" s="20">
         <v>3</v>
       </c>
@@ -4172,10 +4341,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P44" s="55"/>
-      <c r="Q44" s="60"/>
-      <c r="R44" s="55"/>
-      <c r="S44" s="56"/>
+      <c r="P44" s="58"/>
+      <c r="Q44" s="63"/>
+      <c r="R44" s="58"/>
+      <c r="S44" s="59"/>
       <c r="U44" t="s">
         <v>25</v>
       </c>
@@ -4203,7 +4372,7 @@
       <c r="AC44" s="22"/>
       <c r="AD44" s="42"/>
     </row>
-    <row r="45" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="45" spans="11:31">
       <c r="K45" s="20">
         <v>18</v>
       </c>
@@ -4223,10 +4392,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P45" s="55"/>
-      <c r="Q45" s="60"/>
-      <c r="R45" s="55"/>
-      <c r="S45" s="56"/>
+      <c r="P45" s="58"/>
+      <c r="Q45" s="63"/>
+      <c r="R45" s="58"/>
+      <c r="S45" s="59"/>
       <c r="U45" t="s">
         <v>27</v>
       </c>
@@ -4266,7 +4435,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="46" spans="11:31">
       <c r="K46" s="20">
         <v>25</v>
       </c>
@@ -4286,10 +4455,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P46" s="55"/>
-      <c r="Q46" s="60"/>
-      <c r="R46" s="55"/>
-      <c r="S46" s="56"/>
+      <c r="P46" s="58"/>
+      <c r="Q46" s="63"/>
+      <c r="R46" s="58"/>
+      <c r="S46" s="59"/>
       <c r="U46" t="s">
         <v>25</v>
       </c>
@@ -4317,7 +4486,7 @@
       <c r="AC46" s="21"/>
       <c r="AD46" s="33"/>
     </row>
-    <row r="47" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="47" spans="11:31">
       <c r="K47" s="20">
         <v>26</v>
       </c>
@@ -4337,10 +4506,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P47" s="55"/>
-      <c r="Q47" s="60"/>
-      <c r="R47" s="55"/>
-      <c r="S47" s="56"/>
+      <c r="P47" s="58"/>
+      <c r="Q47" s="63"/>
+      <c r="R47" s="58"/>
+      <c r="S47" s="59"/>
       <c r="U47" t="s">
         <v>24</v>
       </c>
@@ -4375,7 +4544,7 @@
       </c>
       <c r="AD47" s="33"/>
     </row>
-    <row r="48" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="48" spans="11:31">
       <c r="K48" s="20">
         <v>27</v>
       </c>
@@ -4395,10 +4564,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P48" s="55"/>
-      <c r="Q48" s="60"/>
-      <c r="R48" s="55"/>
-      <c r="S48" s="56"/>
+      <c r="P48" s="58"/>
+      <c r="Q48" s="63"/>
+      <c r="R48" s="58"/>
+      <c r="S48" s="59"/>
       <c r="U48" t="s">
         <v>25</v>
       </c>
@@ -4426,7 +4595,7 @@
       <c r="AC48" s="21"/>
       <c r="AD48" s="33"/>
     </row>
-    <row r="49" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="49" spans="11:31">
       <c r="K49" s="20">
         <v>28</v>
       </c>
@@ -4446,10 +4615,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P49" s="55"/>
-      <c r="Q49" s="60"/>
-      <c r="R49" s="55"/>
-      <c r="S49" s="56"/>
+      <c r="P49" s="58"/>
+      <c r="Q49" s="63"/>
+      <c r="R49" s="58"/>
+      <c r="S49" s="59"/>
       <c r="U49" t="s">
         <v>24</v>
       </c>
@@ -4484,7 +4653,7 @@
       </c>
       <c r="AD49" s="33"/>
     </row>
-    <row r="50" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="50" spans="11:31">
       <c r="K50" s="20">
         <v>29</v>
       </c>
@@ -4504,10 +4673,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P50" s="55"/>
-      <c r="Q50" s="60"/>
-      <c r="R50" s="55"/>
-      <c r="S50" s="56"/>
+      <c r="P50" s="58"/>
+      <c r="Q50" s="63"/>
+      <c r="R50" s="58"/>
+      <c r="S50" s="59"/>
       <c r="U50" t="s">
         <v>25</v>
       </c>
@@ -4535,7 +4704,7 @@
       <c r="AC50" s="21"/>
       <c r="AD50" s="33"/>
     </row>
-    <row r="51" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="51" spans="11:31">
       <c r="K51" s="20">
         <v>4</v>
       </c>
@@ -4555,10 +4724,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P51" s="55"/>
-      <c r="Q51" s="60"/>
-      <c r="R51" s="55"/>
-      <c r="S51" s="56"/>
+      <c r="P51" s="58"/>
+      <c r="Q51" s="63"/>
+      <c r="R51" s="58"/>
+      <c r="S51" s="59"/>
       <c r="U51" t="s">
         <v>25</v>
       </c>
@@ -4583,7 +4752,7 @@
       </c>
       <c r="AE51" s="20"/>
     </row>
-    <row r="52" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="52" spans="11:31">
       <c r="K52" s="20">
         <v>7</v>
       </c>
@@ -4603,10 +4772,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P52" s="55"/>
-      <c r="Q52" s="60"/>
-      <c r="R52" s="55"/>
-      <c r="S52" s="56"/>
+      <c r="P52" s="58"/>
+      <c r="Q52" s="63"/>
+      <c r="R52" s="58"/>
+      <c r="S52" s="59"/>
       <c r="U52" t="s">
         <v>27</v>
       </c>
@@ -4646,7 +4815,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="53" spans="11:31">
       <c r="K53" s="20">
         <v>8</v>
       </c>
@@ -4666,10 +4835,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P53" s="55"/>
-      <c r="Q53" s="60"/>
-      <c r="R53" s="55"/>
-      <c r="S53" s="56"/>
+      <c r="P53" s="58"/>
+      <c r="Q53" s="63"/>
+      <c r="R53" s="58"/>
+      <c r="S53" s="59"/>
       <c r="U53" t="s">
         <v>25</v>
       </c>
@@ -4697,7 +4866,7 @@
       <c r="AC53" s="21"/>
       <c r="AD53" s="33"/>
     </row>
-    <row r="54" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="54" spans="11:31">
       <c r="K54" s="20">
         <v>12</v>
       </c>
@@ -4717,10 +4886,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P54" s="55"/>
-      <c r="Q54" s="60"/>
-      <c r="R54" s="55"/>
-      <c r="S54" s="56"/>
+      <c r="P54" s="58"/>
+      <c r="Q54" s="63"/>
+      <c r="R54" s="58"/>
+      <c r="S54" s="59"/>
       <c r="U54" s="9" t="s">
         <v>24</v>
       </c>
@@ -4757,7 +4926,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="55" spans="11:31">
       <c r="K55" s="24">
         <v>39</v>
       </c>
@@ -4777,10 +4946,10 @@
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="P55" s="50"/>
-      <c r="Q55" s="54"/>
-      <c r="R55" s="50"/>
-      <c r="S55" s="52"/>
+      <c r="P55" s="53"/>
+      <c r="Q55" s="57"/>
+      <c r="R55" s="53"/>
+      <c r="S55" s="55"/>
       <c r="U55" s="9" t="s">
         <v>25</v>
       </c>
@@ -4808,7 +4977,7 @@
       <c r="AC55" s="21"/>
       <c r="AD55" s="33"/>
     </row>
-    <row r="56" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="56" spans="11:31">
       <c r="U56" s="9" t="s">
         <v>25</v>
       </c>
@@ -4836,7 +5005,7 @@
       <c r="AC56" s="21"/>
       <c r="AD56" s="33"/>
     </row>
-    <row r="57" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="57" spans="11:31">
       <c r="U57" s="9" t="s">
         <v>28</v>
       </c>
@@ -4873,7 +5042,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="58" spans="11:31">
       <c r="U58" s="9" t="s">
         <v>25</v>
       </c>
@@ -4901,7 +5070,7 @@
       <c r="AC58" s="21"/>
       <c r="AD58" s="33"/>
     </row>
-    <row r="59" spans="11:31" x14ac:dyDescent="0.35">
+    <row r="59" spans="11:31">
       <c r="U59" s="9" t="s">
         <v>25</v>
       </c>
@@ -4984,27 +5153,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{563108BE-56B9-49FB-A0AB-612A1346C702}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.4140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -5030,8 +5199,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="61" t="s">
+    <row r="2" spans="1:8">
+      <c r="A2" s="46" t="s">
         <v>63</v>
       </c>
       <c r="B2">
@@ -5059,7 +5228,7 @@
         <v>-5.3715123906329092E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -5085,8 +5254,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="62" t="s">
+    <row r="8" spans="1:8">
+      <c r="A8" s="47" t="s">
         <v>55</v>
       </c>
       <c r="B8" t="s">
@@ -5120,4 +5289,1724 @@
     <ignoredError sqref="A2" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.4140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.4140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="E2">
+        <v>4.1099999999999998E-2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:G34" si="0">D2*F2</f>
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ref="H2:H34" si="1">E2*F2</f>
+        <v>4.1099999999999998E-2</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2:I34" si="2">COMPLEX(G2,H2)</f>
+        <v>0.0035+0.0411i</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ref="J2:J34" si="3">IMAGINARY(IMDIV(1,I2))</f>
+        <v>-24.155725083163901</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>39</v>
+      </c>
+      <c r="D3">
+        <v>1E-3</v>
+      </c>
+      <c r="E3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>1E-3</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="2"/>
+        <v>0.001+0.025i</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="3"/>
+        <v>-39.936102236421704</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="E4">
+        <v>1.5100000000000001E-2</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>1.5100000000000001E-2</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0013+0.0151i</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>-65.737919024815</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E5">
+        <v>8.6E-3</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>8.6E-3</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="2"/>
+        <v>0.007+0.0086i</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>-69.941444372153597</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="E6">
+        <v>2.1299999999999999E-2</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>2.1299999999999999E-2</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0013+0.0213i</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>-46.774122710703203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="E7">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0011+0.0133i</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>-74.677147669848395</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" s="48">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="E8">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0008+0.0128i</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>-77.821011673151702</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>14</v>
+      </c>
+      <c r="D9" s="48">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="E9">
+        <v>1.29E-2</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>1.29E-2</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0008+0.0129i</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>-77.222388506435195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" s="48">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E10">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0002+0.0026i</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>-382.35294117647101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" s="48">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="E11">
+        <v>1.12E-2</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>1.12E-2</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0008+0.0112i</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>-88.832487309644705</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12" s="48">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="E12">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0006+0.0092i</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>-108.235294117647</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13" s="48">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="E13">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0007+0.0082i</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>-121.068950243614</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14" s="48">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E14">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0004+0.0046i</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>-215.75984990619099</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>2.3E-3</v>
+      </c>
+      <c r="E15">
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>2.3E-3</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0023+0.0363i</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>-27.438056508790801</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>39</v>
+      </c>
+      <c r="D16">
+        <v>1E-3</v>
+      </c>
+      <c r="E16">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>1E-3</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="2"/>
+        <v>0.001+0.025i</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>-39.936102236421704</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+      <c r="D17" s="48">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E17">
+        <v>4.3E-3</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>4.3E-3</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0004+0.0043i</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>-230.56300268096501</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>13</v>
+      </c>
+      <c r="D18" s="48">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E18">
+        <v>4.3E-3</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>4.3E-3</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0004+0.0043i</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>-230.56300268096501</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>14</v>
+      </c>
+      <c r="D19" s="48">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="E19">
+        <v>1.01E-2</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>1.01E-2</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0009+0.0101i</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>-98.229916358685102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>1.8E-3</v>
+      </c>
+      <c r="E20">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>1.8E-3</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0018+0.0217i</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="3"/>
+        <v>-45.7680383017316</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21">
+        <v>15</v>
+      </c>
+      <c r="C21">
+        <v>16</v>
+      </c>
+      <c r="D21" s="48">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="E21">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0009+0.0094i</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="3"/>
+        <v>-105.416619939442</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>17</v>
+      </c>
+      <c r="D22" s="48">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="E22">
+        <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0007+0.0089i</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="3"/>
+        <v>-111.668757841907</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>19</v>
+      </c>
+      <c r="D23">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="E23">
+        <v>1.95E-2</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>1.95E-2</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0016+0.0195i</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="3"/>
+        <v>-50.9391081737677</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24">
+        <v>16</v>
+      </c>
+      <c r="C24">
+        <v>21</v>
+      </c>
+      <c r="D24" s="48">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="E24">
+        <v>1.35E-2</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>1.35E-2</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0008+0.0135i</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="3"/>
+        <v>-73.814861392093604</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25">
+        <v>16</v>
+      </c>
+      <c r="C25">
+        <v>24</v>
+      </c>
+      <c r="D25" s="48">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E25">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0003+0.0059i</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="3"/>
+        <v>-169.05444126074499</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26">
+        <v>17</v>
+      </c>
+      <c r="C26">
+        <v>18</v>
+      </c>
+      <c r="D26" s="48">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="E26">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0007+0.0082i</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="3"/>
+        <v>-121.068950243614</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27">
+        <v>17</v>
+      </c>
+      <c r="C27">
+        <v>27</v>
+      </c>
+      <c r="D27">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="E27">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0013+0.0173i</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="3"/>
+        <v>-57.478902252641397</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28">
+        <v>21</v>
+      </c>
+      <c r="C28">
+        <v>22</v>
+      </c>
+      <c r="D28" s="48">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="E28">
+        <v>1.4E-2</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>1.4E-2</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0008+0.014i</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="3"/>
+        <v>-71.196094385679402</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29">
+        <v>22</v>
+      </c>
+      <c r="C29">
+        <v>23</v>
+      </c>
+      <c r="D29" s="48">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="E29">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0006+0.0096i</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="3"/>
+        <v>-103.761348897536</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30">
+        <v>23</v>
+      </c>
+      <c r="C30">
+        <v>24</v>
+      </c>
+      <c r="D30">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="E30">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0022+0.035i</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="3"/>
+        <v>-28.458986534833802</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <v>26</v>
+      </c>
+      <c r="D31">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="E31">
+        <v>3.2300000000000002E-2</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>3.2300000000000002E-2</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0032+0.0323i</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="3"/>
+        <v>-30.658832686302201</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32">
+        <v>26</v>
+      </c>
+      <c r="C32">
+        <v>27</v>
+      </c>
+      <c r="D32">
+        <v>1.4E-3</v>
+      </c>
+      <c r="E32">
+        <v>1.47E-2</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>1.4E-3</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="1"/>
+        <v>1.47E-2</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0014+0.0147i</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="3"/>
+        <v>-67.415730337078699</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33">
+        <v>26</v>
+      </c>
+      <c r="C33">
+        <v>28</v>
+      </c>
+      <c r="D33">
+        <v>4.3E-3</v>
+      </c>
+      <c r="E33">
+        <v>4.7399999999999998E-2</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>4.3E-3</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>4.7399999999999998E-2</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0043+0.0474i</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="3"/>
+        <v>-20.9248427325902</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34">
+        <v>26</v>
+      </c>
+      <c r="C34">
+        <v>29</v>
+      </c>
+      <c r="D34">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="E34">
+        <v>6.25E-2</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="2"/>
+        <v>0.0057+0.0625i</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="3"/>
+        <v>-15.868018706489901</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35">
+        <v>28</v>
+      </c>
+      <c r="C35">
+        <v>29</v>
+      </c>
+      <c r="D35">
+        <v>1.4E-3</v>
+      </c>
+      <c r="E35">
+        <v>1.5100000000000001E-2</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <f>D35*F35</f>
+        <v>1.4E-3</v>
+      </c>
+      <c r="H35">
+        <f>E35*F35</f>
+        <v>1.5100000000000001E-2</v>
+      </c>
+      <c r="I35" t="str">
+        <f>COMPLEX(G35,H35)</f>
+        <v>0.0014+0.0151i</v>
+      </c>
+      <c r="J35">
+        <f>IMAGINARY(IMDIV(1,I35))</f>
+        <v>-65.660738357176996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="K36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37">
+        <v>11</v>
+      </c>
+      <c r="C37">
+        <v>12</v>
+      </c>
+      <c r="D37">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="E37">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <f>D37*F37</f>
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="H37">
+        <f>E37*F37</f>
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="I37" t="str">
+        <f>COMPLEX(G37,H37)</f>
+        <v>0.0016+0.0435i</v>
+      </c>
+      <c r="J37">
+        <f>IMAGINARY(IMDIV(1,I37))</f>
+        <v>-22.957446920799399</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>13</v>
+      </c>
+      <c r="D38">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="E38">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <f t="shared" ref="G38:G39" si="4">D38*F38</f>
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="H38">
+        <f t="shared" ref="H38:H39" si="5">E38*F38</f>
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" ref="I38:I39" si="6">COMPLEX(G38,H38)</f>
+        <v>0.0016+0.0435i</v>
+      </c>
+      <c r="J38">
+        <f t="shared" ref="J38:J39" si="7">IMAGINARY(IMDIV(1,I38))</f>
+        <v>-22.957446920799399</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39">
+        <v>19</v>
+      </c>
+      <c r="C39">
+        <v>20</v>
+      </c>
+      <c r="D39">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="E39">
+        <v>1.38E-2</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="4"/>
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="5"/>
+        <v>1.38E-2</v>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="6"/>
+        <v>0.0007+0.0138i</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="7"/>
+        <v>-72.277798145917302</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" t="s">
+        <v>110</v>
+      </c>
+      <c r="B43">
+        <v>31</v>
+      </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <f t="shared" ref="G43" si="8">D43*F43</f>
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <f t="shared" ref="H43" si="9">E43*F43</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I43" t="str">
+        <f t="shared" ref="I43" si="10">COMPLEX(G43,H43)</f>
+        <v>0.025i</v>
+      </c>
+      <c r="J43">
+        <f t="shared" ref="J43:J51" si="11">IMAGINARY(IMDIV(1,I43))</f>
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44">
+        <v>32</v>
+      </c>
+      <c r="C44">
+        <v>10</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0.02</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <f t="shared" ref="G44:G51" si="12">D44*F44</f>
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <f t="shared" ref="H44:H51" si="13">E44*F44</f>
+        <v>0.02</v>
+      </c>
+      <c r="I44" t="str">
+        <f t="shared" ref="I44:I51" si="14">COMPLEX(G44,H44)</f>
+        <v>0.02i</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="11"/>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45">
+        <v>33</v>
+      </c>
+      <c r="C45">
+        <v>19</v>
+      </c>
+      <c r="D45">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="E45">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="12"/>
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="13"/>
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" si="14"/>
+        <v>0.0007+0.0142i</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="11"/>
+        <v>-70.251818136842601</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46">
+        <v>34</v>
+      </c>
+      <c r="C46">
+        <v>20</v>
+      </c>
+      <c r="D46">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="E46">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="12"/>
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="13"/>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" si="14"/>
+        <v>0.0009+0.018i</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="11"/>
+        <v>-55.417013022998098</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" t="s">
+        <v>114</v>
+      </c>
+      <c r="B47">
+        <v>35</v>
+      </c>
+      <c r="C47">
+        <v>22</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>1.43E-2</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="13"/>
+        <v>1.43E-2</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="14"/>
+        <v>0.0143i</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="11"/>
+        <v>-69.930069930069905</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" t="s">
+        <v>115</v>
+      </c>
+      <c r="B48">
+        <v>36</v>
+      </c>
+      <c r="C48">
+        <v>23</v>
+      </c>
+      <c r="D48">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E48">
+        <v>2.7199999999999998E-2</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="12"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="13"/>
+        <v>2.7199999999999998E-2</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="14"/>
+        <v>0.0005+0.0272i</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="11"/>
+        <v>-36.752286884027598</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" t="s">
+        <v>116</v>
+      </c>
+      <c r="B49">
+        <v>37</v>
+      </c>
+      <c r="C49">
+        <v>25</v>
+      </c>
+      <c r="D49">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="E49">
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="12"/>
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="13"/>
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="14"/>
+        <v>0.0006+0.0232i</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="11"/>
+        <v>-43.074637950241403</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" t="s">
+        <v>117</v>
+      </c>
+      <c r="B50">
+        <v>38</v>
+      </c>
+      <c r="C50">
+        <v>29</v>
+      </c>
+      <c r="D50">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="E50">
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="12"/>
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="13"/>
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="14"/>
+        <v>0.0008+0.0156i</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="11"/>
+        <v>-63.934426229508198</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" t="s">
+        <v>118</v>
+      </c>
+      <c r="B51">
+        <v>30</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>1.8100000000000002E-2</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="13"/>
+        <v>1.8100000000000002E-2</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="14"/>
+        <v>0.0181i</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="11"/>
+        <v>-55.2486187845304</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>